<commit_message>
data files are changed
</commit_message>
<xml_diff>
--- a/Data Files/xlsx files/AMP.xlsx
+++ b/Data Files/xlsx files/AMP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="181">
   <si>
     <t>Description</t>
   </si>
@@ -543,10 +543,22 @@
     <t>Verify the Customer Success text and Css Values</t>
   </si>
   <si>
-    <t>svg_icon</t>
-  </si>
-  <si>
-    <t>path("M11.13 8.524c.34-.27.365-.628.14-1.105a19.186 19.186 0 0 1-.81-1.974 3.194 3.194 0 0 1-.046-1.892c.249-.922.956-1.54 1.934-1.67.709-.094 1.385-.024 1.987.397.898.628 1.065 1.531.96 2.51-.096.908-.437 1.75-.876 2.554-.375.688-.234 1.125.512 1.409.487.185 1.004.294 1.507.438.207.06.421.103.617.186.38.162.661.42.708.848.05.45.191 1.305.237 1.775h-5.28c-.02-.423-.039-.735-.058-.936-.039-.413-.064-.8-.093-1.065-.085-.779-.517-1.156-1.34-1.437a1.79 1.79 0 0 1-.099-.038zM0 12c.09-1.263.097-1.613.298-2.233.125-.386.445-.636.837-.755.558-.169 1.13-.293 1.69-.455a6.36 6.36 0 0 0 .98-.35c.703-.337.82-.825.492-1.522a23.013 23.013 0 0 1-.973-2.369 3.831 3.831 0 0 1-.055-2.269C3.567.942 4.416.2 5.59.044 6.44-.068 7.251.015 7.972.52c1.077.754 1.278 1.837 1.153 3.01-.117 1.09-.525 2.101-1.051 3.065-.451.825-.281 1.349.614 1.69.583.221 1.203.352 1.807.525.248.071.505.123.74.223.456.194.793.504.849 1.018.06.538.087 1.385.142 1.949H0z")</t>
+    <t>icon_value</t>
+  </si>
+  <si>
+    <t>path("M 7 0 C 10.862 0 14 3.138 14 7 S 10.862 14 7 14 S 0 10.862 0 7 S 3.138 0 7 0 Z M 8.918 9.67 L 8.556 7.518 L 10.111 5.988 L 7.959 5.678 L 7 3.732 L 6.04 5.676 L 3.889 5.987 L 5.444 7.517 L 5.082 9.669 L 7 8.659 L 8.918 9.67 Z")</t>
+  </si>
+  <si>
+    <t>path("M 11.13 8.524 C 11.47 8.254 11.495 7.896 11.27 7.419 A 19.186 19.186 0 0 1 10.46 5.445 A 3.194 3.194 0 0 1 10.414 3.553 C 10.663 2.631 11.37 2.013 12.348 1.883 C 13.057 1.789 13.733 1.859 14.335 2.28 C 15.233 2.908 15.4 3.811 15.295 4.79 C 15.199 5.698 14.858 6.54 14.419 7.344 C 14.044 8.032 14.185 8.469 14.931 8.753 C 15.418 8.938 15.935 9.047 16.438 9.191 C 16.645 9.251 16.859 9.294 17.055 9.377 C 17.435 9.539 17.716 9.797 17.763 10.225 C 17.813 10.675 17.954 11.53 18 12 H 12.72 C 12.7 11.577 12.681 11.265 12.662 11.064 C 12.623 10.651 12.598 10.264 12.569 9.999 C 12.484 9.22 12.052 8.843 11.229 8.562 A 1.79 1.79 0 0 1 11.13 8.524 Z M 0 12 C 0.09 10.737 0.097 10.387 0.298 9.767 C 0.423 9.381 0.743 9.131 1.135 9.012 C 1.693 8.843 2.265 8.719 2.825 8.557 A 6.36 6.36 0 0 0 3.805 8.207 C 4.508 7.87 4.625 7.382 4.297 6.685 A 23.013 23.013 0 0 1 3.324 4.316 A 3.831 3.831 0 0 1 3.269 2.047 C 3.567 0.942 4.416 0.2 5.59 0.044 C 6.44 -0.068 7.251 0.015 7.972 0.52 C 9.049 1.274 9.25 2.357 9.125 3.53 C 9.008 4.62 8.6 5.631 8.074 6.595 C 7.623 7.42 7.793 7.944 8.688 8.285 C 9.271 8.506 9.891 8.637 10.495 8.81 C 10.743 8.881 11 8.933 11.235 9.033 C 11.691 9.227 12.028 9.537 12.084 10.051 C 12.144 10.589 12.171 11.436 12.226 12 H 0 Z")</t>
+  </si>
+  <si>
+    <t>path("M 0 8.833 V 0.5 A 0.5 0.5 0 0 1 0.5 0 H 8.833 A 0.5 0.5 0 0 1 9.333 0.5 V 8.833 A 0.5 0.5 0 0 1 8.833 9.333 H 0.5 A 0.5 0.5 0 0 1 0 8.833 Z M 3.468 11.617 V 10.426 H 9.853 A 0.55 0.55 0 0 0 10.425 9.853 V 3.468 H 11.617 V 11.618 H 3.468 Z M 14 14 H 5.851 V 12.809 H 12.236 A 0.55 0.55 0 0 0 12.808 12.236 V 5.851 H 14 V 14 Z")</t>
+  </si>
+  <si>
+    <t>path("M 0.215 10.83 C -0.374 9.51 0.288 7.969 1.686 7.404 L 4.42 6.301 L 6.788 11.608 L 6.518 11.718 L 7.508 13.935 L 4.87 15 L 3.873 12.767 C 2.499 13.216 1.004 12.597 0.443 11.339 L 0.215 10.829 Z M 11.132 0.012 C 11.302 0.052 11.442 0.155 11.509 0.306 L 15.95 10.259 C 15.977 10.319 16.004 10.379 16 10.453 C 16.005 10.719 15.765 10.942 15.485 10.947 L 7.135 11.476 L 4.772 6.15 L 10.664 0.148 A 0.507 0.507 0 0 1 11.132 0.013 Z")</t>
+  </si>
+  <si>
+    <t>path("M 13.838 0.427 C 13.744 0.229 13.526 0.095 13.272 0.034 C 13.242 0.024 13.228 0.025 13.214 0.023 A 1.194 1.194 0 0 0 12.753 0.023 C 12.705 0.028 12.701 0.032 12.695 0.034 C 12.441 0.095 12.223 0.229 12.13 0.427 L 10.596 9.02 L 8.878 4.047 C 8.784 3.848 8.566 3.714 8.311 3.654 C 8.282 3.644 8.271 3.646 8.258 3.644 A 1.175 1.175 0 0 0 7.791 3.644 C 7.746 3.648 7.742 3.652 7.736 3.654 C 7.482 3.714 7.264 3.848 7.17 4.047 L 5.482 8.502 L 3.726 7.067 C 3.712 7.055 3.691 7.051 3.676 7.04 C 3.624 6.998 3.589 6.992 3.561 6.977 A 1.039 1.039 0 0 0 3.387 6.902 C 3.337 6.887 3.288 6.882 3.236 6.875 C 3.178 6.866 3.122 6.857 3.063 6.857 C 3.003 6.857 2.949 6.867 2.891 6.875 C 2.839 6.883 2.789 6.888 2.74 6.902 A 0.966 0.966 0 0 0 2.566 6.977 C 2.536 6.992 2.503 6.998 2.476 7.017 C 2.434 7.051 2.416 7.055 2.401 7.067 L 0.278 9.382 C -0.048 9.649 -0.101 10.242 0.192 10.555 C 0.486 10.868 0.918 10.821 1.242 10.555 L 3.157 8.545 L 5.236 10.243 C 5.561 10.51 6.121 10.533 6.486 10.293 C 6.524 10.27 6.542 10.238 6.572 10.211 A 0.624 0.624 0 0 0 6.716 10.033 C 6.726 10.017 6.744 10.006 6.752 9.989 L 7.985 6.736 L 10.004 12.574 C 10.097 12.773 10.315 12.905 10.569 12.967 C 10.601 12.977 10.615 12.975 10.629 12.977 A 1.142 1.142 0 0 0 11.087 12.977 C 11.137 12.972 11.14 12.969 11.147 12.967 C 11.4 12.905 11.617 12.772 11.712 12.574 L 13.389 3.176 L 14.429 5.216 C 14.588 5.553 15.234 5.671 15.582 5.473 A 0.862 0.862 0 0 0 15.929 4.396 L 13.838 0.427 Z")</t>
   </si>
 </sst>
 </file>
@@ -614,7 +626,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -680,23 +692,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -725,7 +726,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1597,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,6 +1609,7 @@
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" customWidth="1"/>
     <col min="6" max="6" width="32.28515625" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1630,7 +1631,7 @@
       <c r="F1" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="11" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1653,7 +1654,7 @@
       <c r="F2" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1676,6 +1677,9 @@
       <c r="F3" s="10" t="s">
         <v>94</v>
       </c>
+      <c r="G3" s="9" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1696,6 +1700,9 @@
       <c r="F4" s="9" t="s">
         <v>94</v>
       </c>
+      <c r="G4" s="9" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -1716,6 +1723,9 @@
       <c r="F5" s="9" t="s">
         <v>94</v>
       </c>
+      <c r="G5" s="9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1736,6 +1746,9 @@
       <c r="F6" s="9" t="s">
         <v>94</v>
       </c>
+      <c r="G6" s="9" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1756,6 +1769,9 @@
       <c r="F7" s="9" t="s">
         <v>94</v>
       </c>
+      <c r="G7" s="9" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1776,6 +1792,7 @@
       <c r="F8" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1796,6 +1813,7 @@
       <c r="F9" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1816,6 +1834,7 @@
       <c r="F10" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1836,6 +1855,7 @@
       <c r="F11" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -1856,6 +1876,7 @@
       <c r="F12" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1876,6 +1897,7 @@
       <c r="F13" s="10" t="s">
         <v>100</v>
       </c>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1896,6 +1918,7 @@
       <c r="F14" s="10" t="s">
         <v>100</v>
       </c>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1916,6 +1939,7 @@
       <c r="F15" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -1936,8 +1960,9 @@
       <c r="F16" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>125</v>
       </c>
@@ -1956,8 +1981,9 @@
       <c r="F17" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>159</v>
       </c>
@@ -1976,8 +2002,9 @@
       <c r="F18" s="13" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>160</v>
       </c>
@@ -1996,8 +2023,9 @@
       <c r="F19" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>161</v>
       </c>
@@ -2016,8 +2044,9 @@
       <c r="F20" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>162</v>
       </c>
@@ -2036,8 +2065,9 @@
       <c r="F21" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>163</v>
       </c>
@@ -2056,8 +2086,9 @@
       <c r="F22" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>164</v>
       </c>
@@ -2076,8 +2107,9 @@
       <c r="F23" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>165</v>
       </c>
@@ -2096,8 +2128,9 @@
       <c r="F24" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>166</v>
       </c>
@@ -2116,6 +2149,7 @@
       <c r="F25" s="13" t="s">
         <v>146</v>
       </c>
+      <c r="G25" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added the switcher test cases and xlsx file
</commit_message>
<xml_diff>
--- a/Data Files/xlsx files/AMP.xlsx
+++ b/Data Files/xlsx files/AMP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="197">
   <si>
     <t>Description</t>
   </si>
@@ -559,6 +559,54 @@
   </si>
   <si>
     <t>path("M 13.838 0.427 C 13.744 0.229 13.526 0.095 13.272 0.034 C 13.242 0.024 13.228 0.025 13.214 0.023 A 1.194 1.194 0 0 0 12.753 0.023 C 12.705 0.028 12.701 0.032 12.695 0.034 C 12.441 0.095 12.223 0.229 12.13 0.427 L 10.596 9.02 L 8.878 4.047 C 8.784 3.848 8.566 3.714 8.311 3.654 C 8.282 3.644 8.271 3.646 8.258 3.644 A 1.175 1.175 0 0 0 7.791 3.644 C 7.746 3.648 7.742 3.652 7.736 3.654 C 7.482 3.714 7.264 3.848 7.17 4.047 L 5.482 8.502 L 3.726 7.067 C 3.712 7.055 3.691 7.051 3.676 7.04 C 3.624 6.998 3.589 6.992 3.561 6.977 A 1.039 1.039 0 0 0 3.387 6.902 C 3.337 6.887 3.288 6.882 3.236 6.875 C 3.178 6.866 3.122 6.857 3.063 6.857 C 3.003 6.857 2.949 6.867 2.891 6.875 C 2.839 6.883 2.789 6.888 2.74 6.902 A 0.966 0.966 0 0 0 2.566 6.977 C 2.536 6.992 2.503 6.998 2.476 7.017 C 2.434 7.051 2.416 7.055 2.401 7.067 L 0.278 9.382 C -0.048 9.649 -0.101 10.242 0.192 10.555 C 0.486 10.868 0.918 10.821 1.242 10.555 L 3.157 8.545 L 5.236 10.243 C 5.561 10.51 6.121 10.533 6.486 10.293 C 6.524 10.27 6.542 10.238 6.572 10.211 A 0.624 0.624 0 0 0 6.716 10.033 C 6.726 10.017 6.744 10.006 6.752 9.989 L 7.985 6.736 L 10.004 12.574 C 10.097 12.773 10.315 12.905 10.569 12.967 C 10.601 12.977 10.615 12.975 10.629 12.977 A 1.142 1.142 0 0 0 11.087 12.977 C 11.137 12.972 11.14 12.969 11.147 12.967 C 11.4 12.905 11.617 12.772 11.712 12.574 L 13.389 3.176 L 14.429 5.216 C 14.588 5.553 15.234 5.671 15.582 5.473 A 0.862 0.862 0 0 0 15.929 4.396 L 13.838 0.427 Z")</t>
+  </si>
+  <si>
+    <t>TC_025</t>
+  </si>
+  <si>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>Verify the help icon and Css Values</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Verify the Notification icon and Css Values</t>
+  </si>
+  <si>
+    <t>Verify the Profile icon and Css Values</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>var(--cool-grey)</t>
+  </si>
+  <si>
+    <t>Tender</t>
+  </si>
+  <si>
+    <t>Verify the tender icon icon and Css Values</t>
+  </si>
+  <si>
+    <t>path("m 10 0 a 10 10 0 1 1 10 20.002 a 10 10 0 0 1 10 0 z m 9.098 14.777 h 11.028 v 12.925 h 9.098 v 14.777 z m 12.303 5.922 a 4.015 4.015 0 0 0 9.906 5.237 a 3.36 3.36 0 0 0 8.039 5.736 c 7.229 6.255 6.804 7.116 6.762 8.319 h 8.63 c 8.632 7.953 8.74 7.597 8.941 7.292 a 1.15 1.15 0 0 1 10 6.793 c 10.498 6.793 10.84 6.928 11.027 7.198 c 11.216 7.461 11.314 7.778 11.307 8.1 c 11.309 8.38 11.222 8.653 11.057 8.879 c 10.954 9.023 10.827 9.149 10.684 9.253 l 10.218 9.626 a 2.658 2.658 0 0 0 9.346 10.591 c 9.199 11.076 9.126 11.579 9.128 12.085 h 10.872 a 2.8 2.8 0 0 1 10.965 11.339 c 11.041 11.056 11.204 10.805 11.432 10.622 l 11.899 10.279 c 12.247 10.033 12.562 9.739 12.833 9.409 c 13.113 8.997 13.255 8.505 13.237 8.009 a 2.364 2.364 0 0 0 12.303 5.922 z")</t>
+  </si>
+  <si>
+    <t>path("M 4 20 L 5 11 H 0 L 2 0 H 13 L 9 7 H 14 Z")</t>
+  </si>
+  <si>
+    <t>path("M 7.313 2.388 V 1.636 C 7.312 0.733 8.07 0 9 0 C 9.932 0 10.687 0.73 10.687 1.636 V 2.388 C 13.6 3.115 15.75 5.678 15.75 8.728 V 13.091 C 15.75 13.494 16.085 13.818 16.499 13.818 C 17.325 13.818 18 14.468 18 15.273 V 16.365 A 0.371 0.371 0 0 1 17.624 16.727 H 0.376 A 0.368 0.368 0 0 1 0 16.365 V 15.273 C 0 14.472 0.672 13.818 1.501 13.818 A 0.74 0.74 0 0 0 2.25 13.091 V 8.727 C 2.25 5.677 4.402 3.114 7.313 2.387 Z M 6.375 17.455 H 11.625 C 11.625 18.86 10.45 20 9 20 S 6.375 18.86 6.375 17.455 Z")</t>
   </si>
 </sst>
 </file>
@@ -626,7 +674,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -692,12 +740,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -726,6 +785,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1595,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,6 +2210,98 @@
         <v>146</v>
       </c>
       <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>196</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cookies test cases added
</commit_message>
<xml_diff>
--- a/Data Files/xlsx files/AMP.xlsx
+++ b/Data Files/xlsx files/AMP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="197">
   <si>
     <t>Description</t>
   </si>
@@ -549,16 +549,64 @@
     <t>icon_value</t>
   </si>
   <si>
-    <t>path("M0 8.833V.5A.5.5 0 0 1 .5 0h8.333a.5.5 0 0 1 .5.5v8.333a.5.5 0 0 1-.5.5H.5a.5.5 0 0 1-.5-.5zm3.468 2.784v-1.191h6.385a.55.55 0 0 0 .572-.573V3.468h1.192v8.15H3.468zM14 14H5.851v-1.191h6.385a.55.55 0 0 0 .572-.573V5.851H14V14z")</t>
-  </si>
-  <si>
-    <t>path("M.215 10.83c-.589-1.32.073-2.861 1.471-3.426L4.42 6.301l2.368 5.307-.27.11.99 2.217L4.87 15l-.997-2.233c-1.374.449-2.869-.17-3.43-1.428l-.228-.51zM11.132.012c.17.04.31.143.377.294l4.441 9.953c.027.06.054.12.05.194.005.266-.235.489-.515.494l-8.35.529L4.772 6.15 10.664.148a.507.507 0 0 1 .468-.135z")</t>
-  </si>
-  <si>
     <t>path("M 7 0 C 10.862 0 14 3.138 14 7 S 10.862 14 7 14 S 0 10.862 0 7 S 3.138 0 7 0 Z M 8.918 9.67 L 8.556 7.518 L 10.111 5.988 L 7.959 5.678 L 7 3.732 L 6.04 5.676 L 3.889 5.987 L 5.444 7.517 L 5.082 9.669 L 7 8.659 L 8.918 9.67 Z")</t>
   </si>
   <si>
     <t>path("M 13.838 0.427 C 13.744 0.229 13.526 0.095 13.272 0.034 C 13.242 0.024 13.228 0.025 13.214 0.023 A 1.194 1.194 0 0 0 12.753 0.023 C 12.705 0.028 12.701 0.032 12.695 0.034 C 12.441 0.095 12.223 0.229 12.13 0.427 L 10.596 9.02 L 8.878 4.047 C 8.784 3.848 8.566 3.714 8.311 3.654 C 8.282 3.644 8.271 3.646 8.258 3.644 A 1.175 1.175 0 0 0 7.791 3.644 C 7.746 3.648 7.742 3.652 7.736 3.654 C 7.482 3.714 7.264 3.848 7.17 4.047 L 5.482 8.502 L 3.726 7.067 C 3.712 7.055 3.691 7.051 3.676 7.04 C 3.624 6.998 3.589 6.992 3.561 6.977 A 1.039 1.039 0 0 0 3.387 6.902 C 3.337 6.887 3.288 6.882 3.236 6.875 C 3.178 6.866 3.122 6.857 3.063 6.857 C 3.003 6.857 2.949 6.867 2.891 6.875 C 2.839 6.883 2.789 6.888 2.74 6.902 A 0.966 0.966 0 0 0 2.566 6.977 C 2.536 6.992 2.503 6.998 2.476 7.017 C 2.434 7.051 2.416 7.055 2.401 7.067 L 0.278 9.382 C -0.048 9.649 -0.101 10.242 0.192 10.555 C 0.486 10.868 0.918 10.821 1.242 10.555 L 3.157 8.545 L 5.236 10.243 C 5.561 10.51 6.121 10.533 6.486 10.293 C 6.524 10.27 6.542 10.238 6.572 10.211 A 0.624 0.624 0 0 0 6.716 10.033 C 6.726 10.017 6.744 10.006 6.752 9.989 L 7.985 6.736 L 10.004 12.574 C 10.097 12.773 10.315 12.905 10.569 12.967 C 10.601 12.977 10.615 12.975 10.629 12.977 A 1.142 1.142 0 0 0 11.087 12.977 C 11.137 12.972 11.14 12.969 11.147 12.967 C 11.4 12.905 11.617 12.772 11.712 12.574 L 13.389 3.176 L 14.429 5.216 C 14.588 5.553 15.234 5.671 15.582 5.473 A 0.862 0.862 0 0 0 15.929 4.396 L 13.838 0.427 Z")</t>
+  </si>
+  <si>
+    <t>path("M 0 8.833 V 0.5 A 0.5 0.5 0 0 1 0.5 0 H 8.833 A 0.5 0.5 0 0 1 9.333 0.5 V 8.833 A 0.5 0.5 0 0 1 8.833 9.333 H 0.5 A 0.5 0.5 0 0 1 0 8.833 Z M 3.468 11.617 V 10.426 H 9.853 A 0.55 0.55 0 0 0 10.425 9.853 V 3.468 H 11.617 V 11.618 H 3.468 Z M 14 14 H 5.851 V 12.809 H 12.236 A 0.55 0.55 0 0 0 12.808 12.236 V 5.851 H 14 V 14 Z")</t>
+  </si>
+  <si>
+    <t>path("M 0.215 10.83 C -0.374 9.51 0.288 7.969 1.686 7.404 L 4.42 6.301 L 6.788 11.608 L 6.518 11.718 L 7.508 13.935 L 4.87 15 L 3.873 12.767 C 2.499 13.216 1.004 12.597 0.443 11.339 L 0.215 10.829 Z M 11.132 0.012 C 11.302 0.052 11.442 0.155 11.509 0.306 L 15.95 10.259 C 15.977 10.319 16.004 10.379 16 10.453 C 16.005 10.719 15.765 10.942 15.485 10.947 L 7.135 11.476 L 4.772 6.15 L 10.664 0.148 A 0.507 0.507 0 0 1 11.132 0.013 Z")</t>
+  </si>
+  <si>
+    <t>TC_025</t>
+  </si>
+  <si>
+    <t>Verify the help icon and Css Values</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>var(--cool-grey)</t>
+  </si>
+  <si>
+    <t>path("m 10 0 a 10 10 0 1 1 10 20.002 a 10 10 0 0 1 10 0 z m 9.098 14.777 h 11.028 v 12.925 h 9.098 v 14.777 z m 12.303 5.922 a 4.015 4.015 0 0 0 9.906 5.237 a 3.36 3.36 0 0 0 8.039 5.736 c 7.229 6.255 6.804 7.116 6.762 8.319 h 8.63 c 8.632 7.953 8.74 7.597 8.941 7.292 a 1.15 1.15 0 0 1 10 6.793 c 10.498 6.793 10.84 6.928 11.027 7.198 c 11.216 7.461 11.314 7.778 11.307 8.1 c 11.309 8.38 11.222 8.653 11.057 8.879 c 10.954 9.023 10.827 9.149 10.684 9.253 l 10.218 9.626 a 2.658 2.658 0 0 0 9.346 10.591 c 9.199 11.076 9.126 11.579 9.128 12.085 h 10.872 a 2.8 2.8 0 0 1 10.965 11.339 c 11.041 11.056 11.204 10.805 11.432 10.622 l 11.899 10.279 c 12.247 10.033 12.562 9.739 12.833 9.409 c 13.113 8.997 13.255 8.505 13.237 8.009 a 2.364 2.364 0 0 0 12.303 5.922 z")</t>
+  </si>
+  <si>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>Verify the tender icon icon and Css Values</t>
+  </si>
+  <si>
+    <t>Tender</t>
+  </si>
+  <si>
+    <t>path("M 4 20 L 5 11 H 0 L 2 0 H 13 L 9 7 H 14 Z")</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>Verify the Notification icon and Css Values</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>path("M 7.313 2.388 V 1.636 C 7.312 0.733 8.07 0 9 0 C 9.932 0 10.687 0.73 10.687 1.636 V 2.388 C 13.6 3.115 15.75 5.678 15.75 8.728 V 13.091 C 15.75 13.494 16.085 13.818 16.499 13.818 C 17.325 13.818 18 14.468 18 15.273 V 16.365 A 0.371 0.371 0 0 1 17.624 16.727 H 0.376 A 0.368 0.368 0 0 1 0 16.365 V 15.273 C 0 14.472 0.672 13.818 1.501 13.818 A 0.74 0.74 0 0 0 2.25 13.091 V 8.727 C 2.25 5.677 4.402 3.114 7.313 2.387 Z M 6.375 17.455 H 11.625 C 11.625 18.86 10.45 20 9 20 S 6.375 18.86 6.375 17.455 Z")</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>Verify the Profile icon and Css Values</t>
+  </si>
+  <si>
+    <t>Profile</t>
   </si>
 </sst>
 </file>
@@ -708,7 +756,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -737,8 +785,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1609,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,7 +1690,7 @@
       <c r="F1" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1667,8 +1713,8 @@
       <c r="F2" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>179</v>
+      <c r="G2" s="13" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,7 +1736,7 @@
       <c r="F3" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="9" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1713,8 +1759,8 @@
       <c r="F4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>177</v>
+      <c r="G4" s="9" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1736,8 +1782,8 @@
       <c r="F5" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>178</v>
+      <c r="G5" s="9" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1759,8 +1805,8 @@
       <c r="F6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>180</v>
+      <c r="G6" s="9" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1782,8 +1828,8 @@
       <c r="F7" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="15" t="s">
-        <v>175</v>
+      <c r="G7" s="9" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1805,6 +1851,7 @@
       <c r="F8" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1825,6 +1872,7 @@
       <c r="F9" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1845,6 +1893,7 @@
       <c r="F10" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1865,6 +1914,7 @@
       <c r="F11" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -1885,6 +1935,7 @@
       <c r="F12" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1905,6 +1956,7 @@
       <c r="F13" s="10" t="s">
         <v>100</v>
       </c>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1925,6 +1977,7 @@
       <c r="F14" s="10" t="s">
         <v>100</v>
       </c>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1945,6 +1998,7 @@
       <c r="F15" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -1965,8 +2019,9 @@
       <c r="F16" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>125</v>
       </c>
@@ -1985,8 +2040,9 @@
       <c r="F17" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>159</v>
       </c>
@@ -2005,8 +2061,9 @@
       <c r="F18" s="13" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>160</v>
       </c>
@@ -2025,8 +2082,9 @@
       <c r="F19" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>161</v>
       </c>
@@ -2045,8 +2103,9 @@
       <c r="F20" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>162</v>
       </c>
@@ -2065,8 +2124,9 @@
       <c r="F21" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>163</v>
       </c>
@@ -2085,8 +2145,9 @@
       <c r="F22" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>164</v>
       </c>
@@ -2105,8 +2166,9 @@
       <c r="F23" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>165</v>
       </c>
@@ -2125,8 +2187,9 @@
       <c r="F24" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>166</v>
       </c>
@@ -2144,6 +2207,99 @@
       </c>
       <c r="F25" s="13" t="s">
         <v>146</v>
+      </c>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>